<commit_message>
spreadsheet style interface working
</commit_message>
<xml_diff>
--- a/curator-formatter/format/tab_man_template.xlsx
+++ b/curator-formatter/format/tab_man_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhayhurst/Documents/projects/sum-stats-formatter/curator-formatter/format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43524732-AB3E-0042-ADF0-8AF349C5047F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEE727A-E2A7-7640-9089-9321E469A3D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12620" yWindow="-21140" windowWidth="45160" windowHeight="16540" xr2:uid="{97A71DDE-F635-2D4D-A968-2828EFA1FE4A}"/>
+    <workbookView xWindow="-12620" yWindow="-21140" windowWidth="45160" windowHeight="16540" activeTab="2" xr2:uid="{97A71DDE-F635-2D4D-A968-2828EFA1FE4A}"/>
   </bookViews>
   <sheets>
     <sheet name="file" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>fieldSeparator</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>OUT_NAME</t>
+  </si>
+  <si>
+    <t>EXTRACT</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FD132D-8E62-894C-9FF4-EEA12554AFA9}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -591,10 +594,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB4D7B8-2158-DA4F-83FF-7FE5B32CDBFC}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,7 +605,7 @@
     <col min="1" max="3" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -611,6 +614,9 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IN maps to OUT style config
</commit_message>
<xml_diff>
--- a/curator-formatter/format/tab_man_template.xlsx
+++ b/curator-formatter/format/tab_man_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhayhurst/Documents/projects/sum-stats-formatter/curator-formatter/format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEE727A-E2A7-7640-9089-9321E469A3D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A77728F-A024-A84C-B0CF-AABF3FC25A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12620" yWindow="-21140" windowWidth="45160" windowHeight="16540" activeTab="2" xr2:uid="{97A71DDE-F635-2D4D-A968-2828EFA1FE4A}"/>
+    <workbookView xWindow="-12620" yWindow="-21140" windowWidth="45160" windowHeight="16540" activeTab="3" xr2:uid="{97A71DDE-F635-2D4D-A968-2828EFA1FE4A}"/>
   </bookViews>
   <sheets>
     <sheet name="file" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>fieldSeparator</t>
   </si>
@@ -111,10 +111,13 @@
     <t>space=any number of white space characters</t>
   </si>
   <si>
-    <t>OUT_NAME</t>
-  </si>
-  <si>
     <t>EXTRACT</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>OUT</t>
   </si>
 </sst>
 </file>
@@ -596,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB4D7B8-2158-DA4F-83FF-7FE5B32CDBFC}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -616,7 +619,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -628,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA28E48-29B5-D844-A913-0243D0FE8BB6}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -639,10 +642,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mapping style columns config, removed ignore pattern default, added preview
</commit_message>
<xml_diff>
--- a/curator-formatter/format/tab_man_template.xlsx
+++ b/curator-formatter/format/tab_man_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhayhurst/Documents/projects/sum-stats-formatter/curator-formatter/format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A77728F-A024-A84C-B0CF-AABF3FC25A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBDA793-A2D0-2F4B-B70C-EE04808A471C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12620" yWindow="-21140" windowWidth="45160" windowHeight="16540" activeTab="3" xr2:uid="{97A71DDE-F635-2D4D-A968-2828EFA1FE4A}"/>
+    <workbookView xWindow="-9460" yWindow="-26140" windowWidth="45160" windowHeight="16540" xr2:uid="{97A71DDE-F635-2D4D-A968-2828EFA1FE4A}"/>
   </bookViews>
   <sheets>
     <sheet name="file" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>fieldSeparator</t>
   </si>
@@ -45,9 +45,6 @@
     <t>comment</t>
   </si>
   <si>
-    <t>outFileDirectory</t>
-  </si>
-  <si>
     <t>outFilePrefix</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>REPLACE</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>formatted_</t>
   </si>
   <si>
@@ -90,12 +84,6 @@
     <t>BOOL</t>
   </si>
   <si>
-    <t>ignoreFirstNRows</t>
-  </si>
-  <si>
-    <t>COMMENT</t>
-  </si>
-  <si>
     <t>tab</t>
   </si>
   <si>
@@ -118,14 +106,25 @@
   </si>
   <si>
     <t>OUT</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -153,9 +152,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FD132D-8E62-894C-9FF4-EEA12554AFA9}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,57 +485,44 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{758C06F8-963C-7244-A282-525FC4954982}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{758C06F8-963C-7244-A282-525FC4954982}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -553,7 +540,7 @@
           <x14:formula1>
             <xm:f>validation!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B6</xm:sqref>
+          <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -578,16 +565,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -610,16 +597,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA28E48-29B5-D844-A913-0243D0FE8BB6}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -642,10 +629,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -665,15 +652,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -681,7 +668,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -689,12 +676,12 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add log 10 pvalue conversion
</commit_message>
<xml_diff>
--- a/curator-formatter/format/tab_man_template.xlsx
+++ b/curator-formatter/format/tab_man_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhayhurst/Documents/projects/sum-stats-formatter/curator-formatter/format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBDA793-A2D0-2F4B-B70C-EE04808A471C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF548800-D7D1-D241-8E04-8E7A4E05A9C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9460" yWindow="-26140" windowWidth="45160" windowHeight="16540" xr2:uid="{97A71DDE-F635-2D4D-A968-2828EFA1FE4A}"/>
+    <workbookView xWindow="-12320" yWindow="-26140" windowWidth="45160" windowHeight="16540" xr2:uid="{97A71DDE-F635-2D4D-A968-2828EFA1FE4A}"/>
   </bookViews>
   <sheets>
     <sheet name="file" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>fieldSeparator</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>convertLogPvalue</t>
+  </si>
+  <si>
+    <t>set to TRUE if your p_value values need converting from log10(pvalue)</t>
   </si>
 </sst>
 </file>
@@ -470,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FD132D-8E62-894C-9FF4-EEA12554AFA9}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,6 +524,14 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
convert neg log10 values
</commit_message>
<xml_diff>
--- a/curator-formatter/format/tab_man_template.xlsx
+++ b/curator-formatter/format/tab_man_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhayhurst/Documents/projects/sum-stats-formatter/curator-formatter/format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF548800-D7D1-D241-8E04-8E7A4E05A9C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDDAA40-F428-604B-8DBE-BBE8964973D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-12320" yWindow="-26140" windowWidth="45160" windowHeight="16540" xr2:uid="{97A71DDE-F635-2D4D-A968-2828EFA1FE4A}"/>
   </bookViews>
@@ -111,10 +111,10 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>convertLogPvalue</t>
-  </si>
-  <si>
-    <t>set to TRUE if your p_value values need converting from log10(pvalue)</t>
+    <t>convertNegLog10Pvalue</t>
+  </si>
+  <si>
+    <t>set to TRUE if your p_value values need converting from -log10(pvalue)</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>